<commit_message>
Fix up BOM , add positions for assembly
Signed-off-by: Tisham Dhar <whatnickd@gmail.com>
</commit_message>
<xml_diff>
--- a/bom/Onion_Feather_BOM.xlsx
+++ b/bom/Onion_Feather_BOM.xlsx
@@ -37,6 +37,48 @@
     <t xml:space="preserve">Quantity</t>
   </si>
   <si>
+    <t xml:space="preserve">C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0805YD475MAT2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_0805_2012Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8, C17, C19, C20, C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0603C104M4RAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9, C16, C18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0603C105M4PAC7411</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0603C473M4RACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47n</t>
+  </si>
+  <si>
     <t xml:space="preserve">C1, C2, C3, C4, C5, C10, C11, C12, C14, C15</t>
   </si>
   <si>
@@ -46,19 +88,34 @@
     <t xml:space="preserve">10u</t>
   </si>
   <si>
-    <t xml:space="preserve">C_0805_2012Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C8, C17, C19, C20, C21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0603C104M4RAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C_0603_1608Metric</t>
+    <t xml:space="preserve">C13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0805C476M9PACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7, R8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MCT0603MZ0000ZP500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RT0603DRE074K7L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7K</t>
   </si>
   <si>
     <t xml:space="preserve">R3, R4, R5, R6</t>
@@ -68,63 +125,6 @@
   </si>
   <si>
     <t xml:space="preserve">49.9R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R_0603_1608Metric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C9, C16, C18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0603C105M4PAC7411</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1u</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R7, R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCT0603MZ0000ZP500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT0603DRE074K7L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0603YD475MAT2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.7u</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0603C473M4RACTU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0805C476M9PACTU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47u</t>
   </si>
   <si>
     <t xml:space="preserve">L1</t>
@@ -418,7 +418,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,78 +449,78 @@
         <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="E8" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,10 +534,10 @@
         <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,10 +551,10 @@
         <v>34</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>